<commit_message>
Refactor and clean code, rename files, add background color to page one. Change size for question menu in page two
</commit_message>
<xml_diff>
--- a/Final Dataset.xlsx
+++ b/Final Dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,12 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/associateStar</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/fastestDriverTeam</t>
+          <t>http://dbpedia.org/ontology/fastestDriverCountry</t>
         </is>
       </c>
     </row>
@@ -511,11 +506,6 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -545,11 +535,6 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -587,11 +572,6 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -625,11 +605,6 @@
         </is>
       </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Change  place geckoDriver.exe Run case 7
</commit_message>
<xml_diff>
--- a/Final Dataset.xlsx
+++ b/Final Dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,172 +441,352 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/deathPlace</t>
+          <t>test1.csv-COL2</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/parent</t>
+          <t>test1.csv-COL3</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/deathDate</t>
+          <t>test1.csv-COL4</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/birthDate</t>
+          <t>http://dbpedia.org/ontology/percentage</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/birthPlace</t>
+          <t>test1.csv-COL6</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/contest</t>
+          <t>http://dbpedia.org/ontology/populationTotal</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>test2.csv-COL2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>test2.csv-COL3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/weight</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>test3.csv-COL3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>test3.csv-COL4</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>test3.csv-COL5</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Giovanni_Francesco_Guidi_di_Bagno</t>
+          <t>http://dbpedia.org/resource/Terp</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Rome</t>
+          <t>http://dbpedia.org/resource/NAMUR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Colonna_family</t>
+          <t>92136</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1641</t>
+          <t>5100</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1578-10-04 </t>
+          <t>54</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Florence http://dbpedia.org/resource/Grand_Duchy_of_Tuscany </t>
+          <t>http://dbpedia.org/resource/WD</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>1845</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/A1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>92094046</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>92044</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Terp</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>5023</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>4.605</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Giovanni_Doria</t>
+          <t>http://dbpedia.org/resource/Terp</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Palermo</t>
+          <t>http://dbpedia.org/resource/NAMUR</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Giovanni_Andrea_Doria</t>
+          <t>92136</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1642</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>5100</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/WD</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>1845</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>92044</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Terp</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>5023</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>4.605</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Dick_Sheppard_(priest)</t>
+          <t>http://dbpedia.org/resource/Flawinne</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/City_of_London </t>
+          <t>http://dbpedia.org/resource/NAMUR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Edgar_Sheppard </t>
+          <t>92043</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1937-10-31 </t>
+          <t>5020</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1880</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Windsor</t>
+          <t>http://dbpedia.org/resource/FW</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>4491</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>92043</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Flawinne</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>5020</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>6.742</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Claus_Westermann</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Heidelberg http://dbpedia.org/resource/Germany </t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Mother http://dbpedia.org/resource/Father </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2000-06-11 </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1909</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Berlin</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
+          <t>http://dbpedia.org/resource/Citadelle</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>92075</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Citadelle</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>5101</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3.315</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Flawinne</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>92043</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Flawinne</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>5020</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>6.742</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Terp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>92044</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Terp</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>5023</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>4.605</t>
         </is>
       </c>
     </row>

</xml_diff>